<commit_message>
2 ANN model with iterative feature selection algorithm on common   features was added which considers all output columns and best   configuration choice.
</commit_message>
<xml_diff>
--- a/Intersection_Data.xlsx
+++ b/Intersection_Data.xlsx
@@ -451,11 +451,11 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>NARROWFACESECONDARYCOOLINGWATERPRESSUREACTUALMEAN</t>
+          <t>STEELLEVELINMOLD-SETMEAN</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.02911760927683646</v>
+        <v>0.02484936562097117</v>
       </c>
     </row>
     <row r="3">
@@ -464,16 +464,16 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>STEELLEVELINMOLD-SETMEAN</t>
+          <t>NARROWFACESECONDARYCOOLINGWATERPRESSUREACTUALMEAN</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.02255744718641035</v>
+        <v>0.02430368112155793</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -481,20 +481,20 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.01480881377599961</v>
+        <v>0.01622696814615959</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>SEG7+8TOPSECONDARYCOOLINGWATERPRESSUREACTUALMEAN</t>
+          <t>TUNDISHWEIGHTMEAN</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.01320588863852109</v>
+        <v>0.01533290323001619</v>
       </c>
     </row>
     <row r="6">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.01259253407591671</v>
+        <v>0.01415176609373432</v>
       </c>
     </row>
     <row r="7">
@@ -516,37 +516,37 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>TUNDISHWEIGHTMEAN</t>
+          <t>NARROWFACE1WATERFLOWMEAN</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.01164579878968537</v>
+        <v>0.01081853183931805</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>MOLDTAPERPERCENTMEAN</t>
+          <t>SEG9+10+11+12BOTTOMSECONDARYCOOLINGWATERFLOWACTUALMEAN</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.009502756992308658</v>
+        <v>0.009801561493585765</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>PER_NIMEAN</t>
+          <t>LIQUIDUSTEMPMEAN</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.009466015913355781</v>
+        <v>0.009688317844439423</v>
       </c>
     </row>
   </sheetData>

</xml_diff>